<commit_message>
added styling to values page as well as a non-functional button. Also added tasks to spreadsheet and edited formulas
</commit_message>
<xml_diff>
--- a/TasksToComplete(UsingSystem).xlsx
+++ b/TasksToComplete(UsingSystem).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beauw\Documents\GitHub\task_organizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E48022-E7D4-4B4A-9A9D-8E01ECC10603}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A0E9B3-BD09-444C-860C-CD75E0B99727}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15870" yWindow="-105" windowWidth="15990" windowHeight="24840" xr2:uid="{D0EB192E-9ACE-43B8-AF5B-1B4D3617FF40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15990" windowHeight="24840" xr2:uid="{D0EB192E-9ACE-43B8-AF5B-1B4D3617FF40}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <definedName name="Interest_Options">Table1[Personal Interest]</definedName>
     <definedName name="Status_Options">Tasks!$A$2:$A$7</definedName>
     <definedName name="Type_Options">Table1[Type]</definedName>
-    <definedName name="Urgency_Options">Tasks!$E$3:$E$5</definedName>
+    <definedName name="Urgency_Options">Tasks!$E$3:$E$6</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="47">
   <si>
     <t>Urgency</t>
   </si>
@@ -167,9 +167,6 @@
     <t>Python</t>
   </si>
   <si>
-    <t>React</t>
-  </si>
-  <si>
     <t>Javascript/HTML</t>
   </si>
   <si>
@@ -243,6 +240,51 @@
   </si>
   <si>
     <t>Personal Interest</t>
+  </si>
+  <si>
+    <t>Decided to stick with vallinalla JS</t>
+  </si>
+  <si>
+    <t>Save table changes in database</t>
+  </si>
+  <si>
+    <t>Fix JS for laterally dragging of tables</t>
+  </si>
+  <si>
+    <t>Write Calculations from JS</t>
+  </si>
+  <si>
+    <t>"Add" Button</t>
+  </si>
+  <si>
+    <t>"Delete" Button</t>
+  </si>
+  <si>
+    <t>Drag Tables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add a category weighting </t>
+  </si>
+  <si>
+    <t>Make a "Wait" option for tasks</t>
+  </si>
+  <si>
+    <t>Attacht File option for Tasks</t>
+  </si>
+  <si>
+    <t>Timer For Breaks</t>
+  </si>
+  <si>
+    <t>Social Page for Organizational Ideas (videos, articles)</t>
+  </si>
+  <si>
+    <t>reminder every hour about what just happened</t>
+  </si>
+  <si>
+    <t>Email integration</t>
+  </si>
+  <si>
+    <t>Integration</t>
   </si>
 </sst>
 </file>
@@ -409,7 +451,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -426,7 +468,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -434,6 +475,15 @@
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -479,35 +529,17 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF7030A0"/>
+        <color theme="0"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -539,17 +571,26 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="0"/>
+        <color rgb="FF7030A0"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -565,20 +606,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5E868A47-DE23-4011-9E01-05A79D83EB26}" name="Table1" displayName="Table1" ref="C2:H6" totalsRowShown="0">
-  <autoFilter ref="C2:H6" xr:uid="{99700FB1-3C97-4EFD-99B5-8AA3B9A64A9D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5E868A47-DE23-4011-9E01-05A79D83EB26}" name="Table1" displayName="Table1" ref="C2:H7" totalsRowShown="0">
+  <autoFilter ref="C2:H7" xr:uid="{99700FB1-3C97-4EFD-99B5-8AA3B9A64A9D}"/>
   <tableColumns count="6">
-    <tableColumn id="7" xr3:uid="{40172474-8EFA-4AF6-AE33-C13CA6AD9FCB}" name="Type" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{C56B8872-681C-4A83-A844-A47E8B24D599}" name="Type Weight " dataDxfId="6" dataCellStyle="Comma">
-      <calculatedColumnFormula>(ABS((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)/COUNTIF(Table1[Type],"&lt;&gt;"))*D$1</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{40172474-8EFA-4AF6-AE33-C13CA6AD9FCB}" name="Type" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{C56B8872-681C-4A83-A844-A47E8B24D599}" name="Type Weight " dataDxfId="1" dataCellStyle="Comma">
+      <calculatedColumnFormula>(ABS(IF((((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)))/COUNTIF(Table1[Type],"&lt;&gt;"))*D$1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{3960D2BD-ECBB-41F0-981E-3664A49241BE}" name="Urgency" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{14D89874-2270-401E-80C8-C10415CF654C}" name="Urgency Weight" dataDxfId="4" dataCellStyle="Comma">
-      <calculatedColumnFormula>(ABS((ROW()-ROW(E$2))-COUNTIF(Table1[Urgency],"&lt;&gt;")-1)/COUNTIF(Table1[Urgency],"&lt;&gt;"))*F$1</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{14D89874-2270-401E-80C8-C10415CF654C}" name="Urgency Weight" dataDxfId="2" dataCellStyle="Comma">
+      <calculatedColumnFormula>(ABS(IF((((ROW()-ROW(E$2))-COUNTIF(Table1[Urgency],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(E$2))-COUNTIF(Table1[Urgency],"&lt;&gt;")-1)))/COUNTIF(Table1[Urgency],"&lt;&gt;"))*F$1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E5423D4D-AEC2-46C5-BDDC-EF71079C590F}" name="Personal Interest" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{E853A9FB-2928-49DB-AC05-8E4635A41560}" name="Interest Weight" dataDxfId="3">
-      <calculatedColumnFormula>(ABS((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)/COUNTIF(Table1[Personal Interest],"&lt;&gt;"))*H$1</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{E5423D4D-AEC2-46C5-BDDC-EF71079C590F}" name="Personal Interest" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{E853A9FB-2928-49DB-AC05-8E4635A41560}" name="Interest Weight" dataDxfId="0">
+      <calculatedColumnFormula>(ABS(IF((((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)))/COUNTIF(Table1[Personal Interest],"&lt;&gt;"))*H$1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -586,10 +627,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{707AFC97-5499-4218-AB57-9C347DD86A7F}" name="Table2" displayName="Table2" ref="C9:I13" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="C9:I13" xr:uid="{91974E7D-DD51-4A29-81EB-098EEC131316}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C10:H13">
-    <sortCondition descending="1" ref="F9:F13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{707AFC97-5499-4218-AB57-9C347DD86A7F}" name="Table2" displayName="Table2" ref="C10:I27" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="C10:I27" xr:uid="{91974E7D-DD51-4A29-81EB-098EEC131316}">
+    <filterColumn colId="5">
+      <filters blank="1">
+        <filter val="Not Started"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C13:I27">
+    <sortCondition descending="1" ref="F10:F27"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{DFF69775-386F-46E8-A520-F55CB289AEFA}" name="Type"/>
@@ -598,9 +645,9 @@
     <tableColumn id="4" xr3:uid="{109E3EB1-FD7C-4268-A358-CE62204A76E6}" name="Weight" dataCellStyle="Percent">
       <calculatedColumnFormula>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{2ACD96B1-CFAB-4A77-B83C-D2F0F86A8EA4}" name="Task" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{2ACD96B1-CFAB-4A77-B83C-D2F0F86A8EA4}" name="Task" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{F3B46273-2760-48F7-86C0-55414F43850C}" name="Status"/>
-    <tableColumn id="7" xr3:uid="{6B9E9B30-661B-4992-90D3-4414BA426EAD}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{6B9E9B30-661B-4992-90D3-4414BA426EAD}" name="Notes" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -903,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06B6F6B-6B2D-4D97-AF48-5AAF942754D1}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -917,7 +964,7 @@
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
@@ -926,10 +973,10 @@
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" s="7">
         <v>1</v>
@@ -943,13 +990,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>11</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>0</v>
@@ -958,7 +1005,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>2</v>
@@ -966,255 +1013,543 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" s="5">
-        <f>(ABS((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)/COUNTIF(Table1[Type],"&lt;&gt;"))*D$1</f>
+        <f>(ABS(IF((((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)))/COUNTIF(Table1[Type],"&lt;&gt;"))*D$1</f>
         <v>1</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="5">
-        <f>(ABS((ROW()-ROW(E$2))-COUNTIF(Table1[Urgency],"&lt;&gt;")-1)/COUNTIF(Table1[Urgency],"&lt;&gt;"))*F$1</f>
+        <f>(ABS(IF((((ROW()-ROW(E$2))-COUNTIF(Table1[Urgency],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(E$2))-COUNTIF(Table1[Urgency],"&lt;&gt;")-1)))/COUNTIF(Table1[Urgency],"&lt;&gt;"))*F$1</f>
         <v>0.75</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H3" s="5">
-        <f>(ABS((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)/COUNTIF(Table1[Personal Interest],"&lt;&gt;"))*H$1</f>
+        <f>(ABS(IF((((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)))/COUNTIF(Table1[Personal Interest],"&lt;&gt;"))*H$1</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" s="5">
-        <f>(ABS((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)/COUNTIF(Table1[Type],"&lt;&gt;"))*D$1</f>
-        <v>0.75</v>
+        <f>(ABS(IF((((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)))/COUNTIF(Table1[Type],"&lt;&gt;"))*D$1</f>
+        <v>0.8</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="5">
-        <f>(ABS((ROW()-ROW(E$2))-COUNTIF(Table1[Urgency],"&lt;&gt;")-1)/COUNTIF(Table1[Urgency],"&lt;&gt;"))*F$1</f>
+        <f>(ABS(IF((((ROW()-ROW(E$2))-COUNTIF(Table1[Urgency],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(E$2))-COUNTIF(Table1[Urgency],"&lt;&gt;")-1)))/COUNTIF(Table1[Urgency],"&lt;&gt;"))*F$1</f>
         <v>0.5</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>6</v>
       </c>
       <c r="H4" s="6">
-        <f>(ABS((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)/COUNTIF(Table1[Personal Interest],"&lt;&gt;"))*H$1</f>
-        <v>0.375</v>
+        <f>(ABS(IF((((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)))/COUNTIF(Table1[Personal Interest],"&lt;&gt;"))*H$1</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="D5" s="5">
-        <f>(ABS((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)/COUNTIF(Table1[Type],"&lt;&gt;"))*D$1</f>
-        <v>0.5</v>
+        <f>(ABS(IF((((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)))/COUNTIF(Table1[Type],"&lt;&gt;"))*D$1</f>
+        <v>0.6</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="5">
-        <f>(ABS((ROW()-ROW(E$2))-COUNTIF(Table1[Urgency],"&lt;&gt;")-1)/COUNTIF(Table1[Urgency],"&lt;&gt;"))*F$1</f>
+        <f>(ABS(IF((((ROW()-ROW(E$2))-COUNTIF(Table1[Urgency],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(E$2))-COUNTIF(Table1[Urgency],"&lt;&gt;")-1)))/COUNTIF(Table1[Urgency],"&lt;&gt;"))*F$1</f>
         <v>0.25</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H5" s="6">
-        <f>(ABS((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)/COUNTIF(Table1[Personal Interest],"&lt;&gt;"))*H$1</f>
-        <v>0.25</v>
+        <f>(ABS(IF((((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)))/COUNTIF(Table1[Personal Interest],"&lt;&gt;"))*H$1</f>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" s="5">
-        <f>(ABS((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)/COUNTIF(Table1[Type],"&lt;&gt;"))*D$1</f>
-        <v>0.25</v>
+        <f>(ABS(IF((((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)))/COUNTIF(Table1[Type],"&lt;&gt;"))*D$1</f>
+        <v>0.4</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="5">
-        <f>(ABS((ROW()-ROW(E$2))-COUNTIF(Table1[Urgency],"&lt;&gt;")-1)/COUNTIF(Table1[Urgency],"&lt;&gt;"))*F$1</f>
+        <f>(ABS(IF((((ROW()-ROW(E$2))-COUNTIF(Table1[Urgency],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(E$2))-COUNTIF(Table1[Urgency],"&lt;&gt;")-1)))/COUNTIF(Table1[Urgency],"&lt;&gt;"))*F$1</f>
         <v>0</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>8</v>
-      </c>
+      <c r="G6" s="13"/>
       <c r="H6" s="6">
-        <f>(ABS((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)/COUNTIF(Table1[Personal Interest],"&lt;&gt;"))*H$1</f>
-        <v>0.125</v>
+        <f>(ABS(IF((((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)))/COUNTIF(Table1[Personal Interest],"&lt;&gt;"))*H$1</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="5">
+        <f>(ABS(IF((((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)))/COUNTIF(Table1[Type],"&lt;&gt;"))*D$1</f>
+        <v>0.2</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="5">
+        <f>(ABS(IF((((ROW()-ROW(E$2))-COUNTIF(Table1[Urgency],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(E$2))-COUNTIF(Table1[Urgency],"&lt;&gt;")-1)))/COUNTIF(Table1[Urgency],"&lt;&gt;"))*F$1</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="6">
+        <f>(ABS(IF((((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)))/COUNTIF(Table1[Personal Interest],"&lt;&gt;"))*H$1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="2">
+        <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="G11" s="13" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="2">
-        <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="13"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="2">
-        <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>21</v>
-      </c>
       <c r="H11" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
         <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" s="2">
         <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
-        <v>0.58333333333333337</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H12" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I12" s="13"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
       </c>
       <c r="F13" s="2">
         <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
-        <v>0.33333333333333331</v>
+        <v>0.68333333333333324</v>
       </c>
       <c r="G13" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" t="s">
         <v>23</v>
       </c>
-      <c r="H13" t="s">
-        <v>24</v>
-      </c>
       <c r="I13" s="13"/>
     </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="5"/>
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="2">
+        <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="2">
+        <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
+        <v>0.6</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="13"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="2">
+        <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
+        <v>0.6</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="13"/>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="2">
+        <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
+        <v>0.6</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="13"/>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="2">
+        <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
+        <v>0.6</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="13"/>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="2">
+        <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
+        <v>0.6</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="2">
+        <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="13"/>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="2">
+        <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
+        <v>0.4777777777777778</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="13"/>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="2">
+        <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
+        <v>0.3833333333333333</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="13"/>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="2">
+        <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" s="13"/>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="2">
+        <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24" s="13"/>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="2">
+        <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H25" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" s="13"/>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="2">
+        <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H26" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" s="13"/>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="2">
+        <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H27" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C13" xr:uid="{1D88CA36-1020-41D6-A5FF-5776D2F4C8D5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:C27" xr:uid="{1D88CA36-1020-41D6-A5FF-5776D2F4C8D5}">
       <formula1>Type_Options</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:D13" xr:uid="{B2FB62DF-A071-406E-BA3B-892225D6DC14}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:D27" xr:uid="{B2FB62DF-A071-406E-BA3B-892225D6DC14}">
       <formula1>Urgency_Options</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10:E13" xr:uid="{AFDA866C-2043-4AFF-889A-1EEB07EF3914}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11:E27" xr:uid="{AFDA866C-2043-4AFF-889A-1EEB07EF3914}">
       <formula1>Interest_Options</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10:H13" xr:uid="{EB532564-A30A-4A8B-86A4-A09B561C56CB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H11:H27" xr:uid="{EB532564-A30A-4A8B-86A4-A09B561C56CB}">
       <formula1>Status_Options</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
adding working drag and add button in class form
</commit_message>
<xml_diff>
--- a/TasksToComplete(UsingSystem).xlsx
+++ b/TasksToComplete(UsingSystem).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beauw\Documents\GitHub\task_organizer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beauw\Documents\Coding\task_organizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A0E9B3-BD09-444C-860C-CD75E0B99727}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A9B586-ED0B-4A30-9CDD-F1448CD9AB37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15990" windowHeight="24840" xr2:uid="{D0EB192E-9ACE-43B8-AF5B-1B4D3617FF40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D0EB192E-9ACE-43B8-AF5B-1B4D3617FF40}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -144,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="47">
   <si>
     <t>Urgency</t>
   </si>
@@ -361,7 +355,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -410,8 +404,14 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -445,13 +445,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -468,6 +481,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -475,15 +489,6 @@
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -542,6 +547,9 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -560,6 +568,9 @@
       </font>
     </dxf>
     <dxf>
+      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -576,6 +587,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -610,15 +624,15 @@
   <autoFilter ref="C2:H7" xr:uid="{99700FB1-3C97-4EFD-99B5-8AA3B9A64A9D}"/>
   <tableColumns count="6">
     <tableColumn id="7" xr3:uid="{40172474-8EFA-4AF6-AE33-C13CA6AD9FCB}" name="Type" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{C56B8872-681C-4A83-A844-A47E8B24D599}" name="Type Weight " dataDxfId="1" dataCellStyle="Comma">
+    <tableColumn id="8" xr3:uid="{C56B8872-681C-4A83-A844-A47E8B24D599}" name="Type Weight " dataDxfId="7" dataCellStyle="Comma">
       <calculatedColumnFormula>(ABS(IF((((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)))/COUNTIF(Table1[Type],"&lt;&gt;"))*D$1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{3960D2BD-ECBB-41F0-981E-3664A49241BE}" name="Urgency" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{14D89874-2270-401E-80C8-C10415CF654C}" name="Urgency Weight" dataDxfId="2" dataCellStyle="Comma">
+    <tableColumn id="3" xr3:uid="{3960D2BD-ECBB-41F0-981E-3664A49241BE}" name="Urgency" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{14D89874-2270-401E-80C8-C10415CF654C}" name="Urgency Weight" dataDxfId="5" dataCellStyle="Comma">
       <calculatedColumnFormula>(ABS(IF((((ROW()-ROW(E$2))-COUNTIF(Table1[Urgency],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(E$2))-COUNTIF(Table1[Urgency],"&lt;&gt;")-1)))/COUNTIF(Table1[Urgency],"&lt;&gt;"))*F$1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E5423D4D-AEC2-46C5-BDDC-EF71079C590F}" name="Personal Interest" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{E853A9FB-2928-49DB-AC05-8E4635A41560}" name="Interest Weight" dataDxfId="0">
+    <tableColumn id="5" xr3:uid="{E5423D4D-AEC2-46C5-BDDC-EF71079C590F}" name="Personal Interest" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{E853A9FB-2928-49DB-AC05-8E4635A41560}" name="Interest Weight" dataDxfId="3">
       <calculatedColumnFormula>(ABS(IF((((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)))/COUNTIF(Table1[Personal Interest],"&lt;&gt;"))*H$1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -627,7 +641,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{707AFC97-5499-4218-AB57-9C347DD86A7F}" name="Table2" displayName="Table2" ref="C10:I27" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{707AFC97-5499-4218-AB57-9C347DD86A7F}" name="Table2" displayName="Table2" ref="C10:I27" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="C10:I27" xr:uid="{91974E7D-DD51-4A29-81EB-098EEC131316}">
     <filterColumn colId="5">
       <filters blank="1">
@@ -645,9 +659,9 @@
     <tableColumn id="4" xr3:uid="{109E3EB1-FD7C-4268-A358-CE62204A76E6}" name="Weight" dataCellStyle="Percent">
       <calculatedColumnFormula>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{2ACD96B1-CFAB-4A77-B83C-D2F0F86A8EA4}" name="Task" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{2ACD96B1-CFAB-4A77-B83C-D2F0F86A8EA4}" name="Task" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{F3B46273-2760-48F7-86C0-55414F43850C}" name="Status"/>
-    <tableColumn id="7" xr3:uid="{6B9E9B30-661B-4992-90D3-4414BA426EAD}" name="Notes" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{6B9E9B30-661B-4992-90D3-4414BA426EAD}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -950,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06B6F6B-6B2D-4D97-AF48-5AAF942754D1}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -971,7 +985,7 @@
     <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>21</v>
       </c>
@@ -988,7 +1002,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1011,11 +1025,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="5">
@@ -1037,7 +1051,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1063,7 +1077,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1089,11 +1103,11 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="5">
@@ -1110,8 +1124,11 @@
         <f>(ABS(IF((((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)))/COUNTIF(Table1[Personal Interest],"&lt;&gt;"))*H$1</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L6" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1133,12 +1150,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" s="9" t="s">
         <v>9</v>
       </c>
@@ -1161,7 +1178,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>13</v>
       </c>
@@ -1183,7 +1200,7 @@
       </c>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>13</v>
       </c>
@@ -1205,7 +1222,7 @@
       </c>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>11</v>
       </c>
@@ -1227,7 +1244,7 @@
       </c>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>12</v>
       </c>
@@ -1251,7 +1268,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>11</v>
       </c>
@@ -1273,7 +1290,7 @@
       </c>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
adding completed classes and base from last build
</commit_message>
<xml_diff>
--- a/TasksToComplete(UsingSystem).xlsx
+++ b/TasksToComplete(UsingSystem).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beauw\Documents\Coding\task_organizer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beauw\Documents\GitHub\task_organizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A9B586-ED0B-4A30-9CDD-F1448CD9AB37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B831F7B2-610B-49D6-9318-0B17BEDB6695}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D0EB192E-9ACE-43B8-AF5B-1B4D3617FF40}"/>
+    <workbookView xWindow="15630" yWindow="-120" windowWidth="15990" windowHeight="24840" xr2:uid="{D0EB192E-9ACE-43B8-AF5B-1B4D3617FF40}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="50">
   <si>
     <t>Urgency</t>
   </si>
@@ -245,9 +245,6 @@
     <t>Fix JS for laterally dragging of tables</t>
   </si>
   <si>
-    <t>Write Calculations from JS</t>
-  </si>
-  <si>
     <t>"Add" Button</t>
   </si>
   <si>
@@ -257,9 +254,6 @@
     <t>Drag Tables</t>
   </si>
   <si>
-    <t xml:space="preserve">Add a category weighting </t>
-  </si>
-  <si>
     <t>Make a "Wait" option for tasks</t>
   </si>
   <si>
@@ -279,6 +273,21 @@
   </si>
   <si>
     <t>Integration</t>
+  </si>
+  <si>
+    <t>Task Calculations</t>
+  </si>
+  <si>
+    <t>Minimum Viable Product</t>
+  </si>
+  <si>
+    <t>Steps HTML</t>
+  </si>
+  <si>
+    <t>Tonight</t>
+  </si>
+  <si>
+    <t>Due Date</t>
   </si>
 </sst>
 </file>
@@ -464,7 +473,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -482,6 +491,10 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -620,8 +633,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5E868A47-DE23-4011-9E01-05A79D83EB26}" name="Table1" displayName="Table1" ref="C2:H7" totalsRowShown="0">
-  <autoFilter ref="C2:H7" xr:uid="{99700FB1-3C97-4EFD-99B5-8AA3B9A64A9D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5E868A47-DE23-4011-9E01-05A79D83EB26}" name="Table1" displayName="Table1" ref="C2:H8" totalsRowShown="0">
+  <autoFilter ref="C2:H8" xr:uid="{99700FB1-3C97-4EFD-99B5-8AA3B9A64A9D}"/>
   <tableColumns count="6">
     <tableColumn id="7" xr3:uid="{40172474-8EFA-4AF6-AE33-C13CA6AD9FCB}" name="Type" dataDxfId="8"/>
     <tableColumn id="8" xr3:uid="{C56B8872-681C-4A83-A844-A47E8B24D599}" name="Type Weight " dataDxfId="7" dataCellStyle="Comma">
@@ -641,18 +654,19 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{707AFC97-5499-4218-AB57-9C347DD86A7F}" name="Table2" displayName="Table2" ref="C10:I27" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="C10:I27" xr:uid="{91974E7D-DD51-4A29-81EB-098EEC131316}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{707AFC97-5499-4218-AB57-9C347DD86A7F}" name="Table2" displayName="Table2" ref="C11:J28" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="C11:J28" xr:uid="{91974E7D-DD51-4A29-81EB-098EEC131316}">
     <filterColumn colId="5">
-      <filters blank="1">
+      <filters>
+        <filter val="Development"/>
         <filter val="Not Started"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C13:I27">
-    <sortCondition descending="1" ref="F10:F27"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C16:I28">
+    <sortCondition descending="1" ref="F11:F28"/>
   </sortState>
-  <tableColumns count="7">
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{DFF69775-386F-46E8-A520-F55CB289AEFA}" name="Type"/>
     <tableColumn id="2" xr3:uid="{EB78546C-5E5C-4FE9-A712-B665990AB1CC}" name="Urgency"/>
     <tableColumn id="3" xr3:uid="{5721D9DB-6140-45FF-9BEC-4E3A33246645}" name="Personal Interest"/>
@@ -662,6 +676,7 @@
     <tableColumn id="5" xr3:uid="{2ACD96B1-CFAB-4A77-B83C-D2F0F86A8EA4}" name="Task" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{F3B46273-2760-48F7-86C0-55414F43850C}" name="Status"/>
     <tableColumn id="7" xr3:uid="{6B9E9B30-661B-4992-90D3-4414BA426EAD}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{9D6ED705-780C-497E-8586-368D79B7E9E9}" name="Due Date"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -964,10 +979,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06B6F6B-6B2D-4D97-AF48-5AAF942754D1}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1029,8 +1044,8 @@
       <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>13</v>
+      <c r="C3" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="D3" s="5">
         <f>(ABS(IF((((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)))/COUNTIF(Table1[Type],"&lt;&gt;"))*D$1</f>
@@ -1044,7 +1059,7 @@
         <v>0.75</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H3" s="5">
         <f>(ABS(IF((((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)))/COUNTIF(Table1[Personal Interest],"&lt;&gt;"))*H$1</f>
@@ -1060,7 +1075,7 @@
       </c>
       <c r="D4" s="5">
         <f>(ABS(IF((((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)))/COUNTIF(Table1[Type],"&lt;&gt;"))*D$1</f>
-        <v>0.8</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>4</v>
@@ -1070,7 +1085,7 @@
         <v>0.5</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H4" s="6">
         <f>(ABS(IF((((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)))/COUNTIF(Table1[Personal Interest],"&lt;&gt;"))*H$1</f>
@@ -1082,11 +1097,11 @@
         <v>26</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" s="5">
         <f>(ABS(IF((((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)))/COUNTIF(Table1[Type],"&lt;&gt;"))*D$1</f>
-        <v>0.6</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>5</v>
@@ -1112,7 +1127,7 @@
       </c>
       <c r="D6" s="5">
         <f>(ABS(IF((((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)))/COUNTIF(Table1[Type],"&lt;&gt;"))*D$1</f>
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="5">
@@ -1137,7 +1152,7 @@
       </c>
       <c r="D7" s="5">
         <f>(ABS(IF((((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)))/COUNTIF(Table1[Type],"&lt;&gt;"))*D$1</f>
-        <v>0.2</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="5">
@@ -1150,127 +1165,125 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C9" s="3" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="15">
+        <f>(ABS(IF((((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(C$2))-COUNTIF(Table1[Type],"&lt;&gt;")-1)))/COUNTIF(Table1[Type],"&lt;&gt;"))*D$1</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="15">
+        <f>(ABS(IF((((ROW()-ROW(E$2))-COUNTIF(Table1[Urgency],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(E$2))-COUNTIF(Table1[Urgency],"&lt;&gt;")-1)))/COUNTIF(Table1[Urgency],"&lt;&gt;"))*F$1</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="6">
+        <f>(ABS(IF((((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)*-1)&lt;0,0,((ROW()-ROW(G$2))-COUNTIF(Table1[Personal Interest],"&lt;&gt;")-1)))/COUNTIF(Table1[Personal Interest],"&lt;&gt;"))*H$1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C10" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C10" s="9" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D11" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="2">
-        <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
-        <v>0.63888888888888895</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="13"/>
+      <c r="J11" s="4" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="2">
         <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
-        <v>0.55555555555555558</v>
+        <v>0.3611111111111111</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H12" t="s">
         <v>28</v>
       </c>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F13" s="2">
         <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
-        <v>0.68333333333333324</v>
+        <v>0.27777777777777773</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="H13" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="I13" s="13"/>
     </row>
     <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
       </c>
       <c r="F14" s="2">
         <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
-        <v>0.39999999999999997</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="H14" t="s">
         <v>28</v>
       </c>
-      <c r="I14" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I14" s="13"/>
+    </row>
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
@@ -1280,19 +1293,21 @@
       </c>
       <c r="F15" s="2">
         <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
-        <v>0.6</v>
+        <v>0.38888888888888884</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="H15" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15" s="13"/>
+        <v>28</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="D16" t="s">
         <v>4</v>
@@ -1302,19 +1317,22 @@
       </c>
       <c r="F16" s="2">
         <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
-        <v>0.6</v>
+        <v>0.61111111111111105</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="H16" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="13"/>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="I16" s="16"/>
+      <c r="J16" s="17">
+        <v>44088</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="D17" t="s">
         <v>4</v>
@@ -1324,17 +1342,20 @@
       </c>
       <c r="F17" s="2">
         <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
-        <v>0.6</v>
+        <v>0.61111111111111105</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="H17" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="13"/>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="I17" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17" s="18"/>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>11</v>
       </c>
@@ -1346,17 +1367,18 @@
       </c>
       <c r="F18" s="2">
         <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
-        <v>0.6</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H18" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I18" s="13"/>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="18"/>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>11</v>
       </c>
@@ -1368,41 +1390,43 @@
       </c>
       <c r="F19" s="2">
         <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
-        <v>0.6</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H19" t="s">
         <v>23</v>
       </c>
       <c r="I19" s="13"/>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="18"/>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D20" t="s">
         <v>4</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" s="2">
         <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
         <v>0.55555555555555558</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="H20" t="s">
         <v>23</v>
       </c>
       <c r="I20" s="13"/>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="18"/>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D21" t="s">
         <v>4</v>
@@ -1412,17 +1436,18 @@
       </c>
       <c r="F21" s="2">
         <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
-        <v>0.4777777777777778</v>
+        <v>0.55555555555555547</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H21" t="s">
         <v>23</v>
       </c>
       <c r="I21" s="13"/>
-    </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="18"/>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>14</v>
       </c>
@@ -1434,7 +1459,7 @@
       </c>
       <c r="F22" s="2">
         <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
-        <v>0.3833333333333333</v>
+        <v>0.3611111111111111</v>
       </c>
       <c r="G22" s="13" t="s">
         <v>34</v>
@@ -1443,8 +1468,9 @@
         <v>23</v>
       </c>
       <c r="I22" s="13"/>
-    </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="18"/>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>12</v>
       </c>
@@ -1456,17 +1482,18 @@
       </c>
       <c r="F23" s="2">
         <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
-        <v>0.31666666666666665</v>
+        <v>0.30555555555555552</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H23" t="s">
         <v>23</v>
       </c>
       <c r="I23" s="13"/>
-    </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="18"/>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>12</v>
       </c>
@@ -1478,17 +1505,18 @@
       </c>
       <c r="F24" s="2">
         <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
-        <v>0.31666666666666665</v>
+        <v>0.30555555555555552</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H24" t="s">
         <v>23</v>
       </c>
       <c r="I24" s="13"/>
-    </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="18"/>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>12</v>
       </c>
@@ -1500,17 +1528,18 @@
       </c>
       <c r="F25" s="2">
         <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
-        <v>0.31666666666666665</v>
+        <v>0.30555555555555552</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H25" t="s">
         <v>23</v>
       </c>
       <c r="I25" s="13"/>
-    </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="18"/>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>12</v>
       </c>
@@ -1522,17 +1551,18 @@
       </c>
       <c r="F26" s="2">
         <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
-        <v>0.31666666666666665</v>
+        <v>0.30555555555555552</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H26" t="s">
         <v>23</v>
       </c>
       <c r="I26" s="13"/>
-    </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="18"/>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>12</v>
       </c>
@@ -1544,29 +1574,53 @@
       </c>
       <c r="F27" s="2">
         <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
-        <v>0.31666666666666665</v>
+        <v>0.30555555555555552</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H27" t="s">
         <v>23</v>
       </c>
       <c r="I27" s="13"/>
+      <c r="J27" s="18"/>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="2">
+        <f>SUM(VLOOKUP(Table2[[#This Row],[Type]],Table1[[Type]:[Type Weight ]],2,FALSE),VLOOKUP(Table2[[#This Row],[Urgency]],Table1[[Urgency]:[Urgency Weight]],2,FALSE),VLOOKUP(Table2[[#This Row],[Personal Interest]],Table1[[Personal Interest]:[Interest Weight]],2,FALSE))/COUNTIF(Table2[[#This Row],[Type]:[Personal Interest]],"&lt;&gt;")</f>
+        <v>0.19444444444444442</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I28" s="13"/>
+      <c r="J28" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:C27" xr:uid="{1D88CA36-1020-41D6-A5FF-5776D2F4C8D5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12:C28" xr:uid="{1D88CA36-1020-41D6-A5FF-5776D2F4C8D5}">
       <formula1>Type_Options</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:D27" xr:uid="{B2FB62DF-A071-406E-BA3B-892225D6DC14}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12:D28" xr:uid="{B2FB62DF-A071-406E-BA3B-892225D6DC14}">
       <formula1>Urgency_Options</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11:E27" xr:uid="{AFDA866C-2043-4AFF-889A-1EEB07EF3914}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12:E28" xr:uid="{AFDA866C-2043-4AFF-889A-1EEB07EF3914}">
       <formula1>Interest_Options</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H11:H27" xr:uid="{EB532564-A30A-4A8B-86A4-A09B561C56CB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H12:H28" xr:uid="{EB532564-A30A-4A8B-86A4-A09B561C56CB}">
       <formula1>Status_Options</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>